<commit_message>
Entrega Final Reto 2
</commit_message>
<xml_diff>
--- a/Docs/Reto2_Gráficas_EntregaFinal.xlsx
+++ b/Docs/Reto2_Gráficas_EntregaFinal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianadiaz/Downloads/Reto 2/Reto2-G07/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/ESTRUCTURA DE DATOS/LABORATORIOS/Reto2-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411C537C-4ACA-7E43-AD96-E748ABDC5FAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas datos" sheetId="1" r:id="rId1"/>
@@ -19,16 +20,16 @@
     <sheet name="Requerimiento 3" sheetId="10" r:id="rId5"/>
     <sheet name="Requerimiento 4" sheetId="11" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -197,15 +198,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Millares [0]" xfId="5" builtinId="6"/>
+    <cellStyle name="Comma [0]" xfId="5" builtinId="6"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -222,9 +223,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -273,8 +274,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -302,7 +303,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -354,7 +355,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -380,7 +380,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -392,25 +392,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -422,22 +422,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4141.647</c:v>
+                  <c:v>4141.6469999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8380.584999999999</c:v>
+                  <c:v>8380.5849999999991</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>17192.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26679.294</c:v>
+                  <c:v>26679.294000000002</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>44319.38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72465.944</c:v>
+                  <c:v>72465.944000000003</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>89600.37</c:v>
@@ -446,6 +446,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F75D-BD49-B335-97EC77C36B68}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -543,10 +548,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -580,7 +586,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-936636128"/>
@@ -639,7 +645,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -665,7 +670,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -703,7 +708,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-936592880"/>
@@ -724,10 +729,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.263045656195262"/>
-          <c:y val="0.905458486992923"/>
-          <c:w val="0.54043659043659"/>
-          <c:h val="0.0597313864247982"/>
+          <c:x val="0.26304565619526199"/>
+          <c:y val="0.90545848699292297"/>
+          <c:w val="0.54043659043658998"/>
+          <c:h val="5.9731386424798201E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -755,7 +760,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -785,7 +790,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -797,9 +802,9 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -841,7 +846,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.363947026782942"/>
-          <c:y val="0.0369274450613244"/>
+          <c:y val="3.69274450613244E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -869,7 +874,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -882,8 +887,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.114765472864279"/>
           <c:y val="0.110160857908847"/>
-          <c:w val="0.849678971580165"/>
-          <c:h val="0.692041755504422"/>
+          <c:w val="0.84967897158016503"/>
+          <c:h val="0.69204175550442204"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -939,7 +944,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -965,7 +969,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -977,25 +981,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1007,7 +1011,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="0.00">
-                  <c:v>2.715</c:v>
+                  <c:v>2.7149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.41</c:v>
@@ -1022,15 +1026,20 @@
                   <c:v>23.41</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
-                  <c:v>37.559</c:v>
+                  <c:v>37.558999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>47.566</c:v>
+                  <c:v>47.566000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67FE-DC44-AC65-F06E06D06B2D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1099,8 +1108,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.466905144921401"/>
-              <c:y val="0.86393658567478"/>
+              <c:x val="0.46690514492140101"/>
+              <c:y val="0.86393658567478004"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1128,7 +1137,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1166,7 +1175,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-937069440"/>
@@ -1177,7 +1186,7 @@
         <c:axId val="-937069440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.0"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1230,8 +1239,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.014336917562724"/>
-              <c:y val="0.3058533702054"/>
+              <c:x val="1.4336917562724E-2"/>
+              <c:y val="0.30585337020539999"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1259,7 +1268,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1297,7 +1306,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-878439888"/>
@@ -1318,10 +1327,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.333672000677335"/>
-          <c:y val="0.927948745012772"/>
-          <c:w val="0.433602150537634"/>
-          <c:h val="0.0506035338076038"/>
+          <c:x val="0.33367200067733499"/>
+          <c:y val="0.92794874501277202"/>
+          <c:w val="0.43360215053763401"/>
+          <c:h val="5.0603533807603802E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1349,7 +1358,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1379,7 +1388,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1391,9 +1400,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1434,8 +1443,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1463,7 +1472,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1523,7 +1532,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1549,7 +1557,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1561,25 +1569,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1591,30 +1599,35 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>66699.886</c:v>
+                  <c:v>66699.885999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>133142.915</c:v>
+                  <c:v>133142.91500000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>265840.211</c:v>
+                  <c:v>265840.21100000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>398593.565</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>665719.883</c:v>
+                  <c:v>665719.88300000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.064423906E6</c:v>
+                  <c:v>1064423.906</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.330399157E6</c:v>
+                  <c:v>1330399.1569999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AB8B-4F44-A394-457F720675FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1683,8 +1696,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.429602572826545"/>
-              <c:y val="0.83829617092256"/>
+              <c:x val="0.42960257282654501"/>
+              <c:y val="0.83829617092256004"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1712,10 +1725,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1749,7 +1763,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-906128512"/>
@@ -1808,7 +1822,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1834,7 +1847,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1872,7 +1885,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-909285536"/>
@@ -1894,9 +1907,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.236676873724118"/>
-          <c:y val="0.906931096229794"/>
-          <c:w val="0.534876543209877"/>
-          <c:h val="0.0588009909976206"/>
+          <c:y val="0.90693109622979395"/>
+          <c:w val="0.53487654320987699"/>
+          <c:h val="5.8800990997620602E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1924,7 +1937,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1954,7 +1967,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1966,9 +1979,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2009,8 +2022,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2038,7 +2051,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2051,8 +2064,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.123233701945345"/>
           <c:y val="0.119447674418605"/>
-          <c:w val="0.840295709819361"/>
-          <c:h val="0.666080159311481"/>
+          <c:w val="0.84029570981936097"/>
+          <c:h val="0.66608015931148101"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2108,7 +2121,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2134,7 +2146,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2146,25 +2158,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2182,7 +2194,7 @@
                   <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.469</c:v>
+                  <c:v>14.468999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.352</c:v>
@@ -2191,15 +2203,20 @@
                   <c:v>15.57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.453</c:v>
+                  <c:v>16.452999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.672</c:v>
+                  <c:v>16.672000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A35-954A-AA5D-0B85DDD8AFDC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2268,8 +2285,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.428256137100509"/>
-              <c:y val="0.863227430873466"/>
+              <c:x val="0.42825613710050903"/>
+              <c:y val="0.86322743087346598"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2297,10 +2314,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2334,7 +2352,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-909288672"/>
@@ -2345,7 +2363,7 @@
         <c:axId val="-909288672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="13.0"/>
+          <c:min val="13"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2398,8 +2416,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0294117647058823"/>
-              <c:y val="0.289486357809925"/>
+              <c:x val="2.94117647058823E-2"/>
+              <c:y val="0.28948635780992499"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2427,7 +2445,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2465,7 +2483,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-909305216"/>
@@ -2482,7 +2500,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2508,7 +2525,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2538,7 +2555,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2550,9 +2567,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2601,8 +2618,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2630,7 +2647,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2641,9 +2658,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12656666763518"/>
+          <c:x val="0.12656666763518001"/>
           <c:y val="0.121568047337278"/>
-          <c:w val="0.836828166313159"/>
+          <c:w val="0.83682816631315904"/>
           <c:h val="0.660152588174999"/>
         </c:manualLayout>
       </c:layout>
@@ -2700,7 +2717,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2726,7 +2742,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2738,25 +2754,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2771,13 +2787,13 @@
                   <c:v>14.884</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.248</c:v>
+                  <c:v>24.248000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56.505</c:v>
+                  <c:v>56.505000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.015</c:v>
+                  <c:v>77.015000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>126.596</c:v>
@@ -2786,12 +2802,17 @@
                   <c:v>260.387</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>290.119</c:v>
+                  <c:v>290.11900000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EDE7-3E48-B776-C9276C4988BB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2860,8 +2881,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.428106894848476"/>
-              <c:y val="0.85949471182966"/>
+              <c:x val="0.42810689484847603"/>
+              <c:y val="0.85949471182965997"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2889,10 +2910,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2926,7 +2948,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222632752"/>
@@ -2989,8 +3011,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0239852398523985"/>
-              <c:y val="0.290779015049154"/>
+              <c:x val="2.3985239852398501E-2"/>
+              <c:y val="0.29077901504915399"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3018,7 +3040,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3056,7 +3078,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222636144"/>
@@ -3073,7 +3095,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3099,7 +3120,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3129,7 +3150,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3141,9 +3162,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3192,8 +3213,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.373041577746707"/>
-          <c:y val="0.0372495329975645"/>
+          <c:x val="0.37304157774670699"/>
+          <c:y val="3.7249532997564498E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3221,7 +3242,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3232,10 +3253,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.140484362351902"/>
-          <c:y val="0.121928783382789"/>
-          <c:w val="0.822431525498565"/>
-          <c:h val="0.710483178239084"/>
+          <c:x val="0.14048436235190201"/>
+          <c:y val="0.12192878338278899"/>
+          <c:w val="0.82243152549856502"/>
+          <c:h val="0.71048317823908402"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3291,7 +3312,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3317,7 +3337,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3329,25 +3349,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3359,10 +3379,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>137.605</c:v>
+                  <c:v>137.60499999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>310.732</c:v>
+                  <c:v>310.73200000000003</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>658.91</c:v>
@@ -3371,18 +3391,23 @@
                   <c:v>1204.711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2114.303</c:v>
+                  <c:v>2114.3029999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3718.283</c:v>
+                  <c:v>3718.2829999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4356.169</c:v>
+                  <c:v>4356.1689999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0458-B64A-96B3-8369C3070C62}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3451,8 +3476,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.448136581058209"/>
-              <c:y val="0.881263869005011"/>
+              <c:x val="0.44813658105820903"/>
+              <c:y val="0.88126386900501097"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3480,10 +3505,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3517,7 +3543,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222457440"/>
@@ -3580,8 +3606,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0205607476635514"/>
-              <c:y val="0.330032243744013"/>
+              <c:x val="2.0560747663551399E-2"/>
+              <c:y val="0.33003224374401302"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3609,7 +3635,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3647,7 +3673,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222460832"/>
@@ -3668,10 +3694,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.292570019869012"/>
-          <c:y val="0.926491141732284"/>
-          <c:w val="0.452242990654206"/>
-          <c:h val="0.0536224946313529"/>
+          <c:x val="0.29257001986901199"/>
+          <c:y val="0.92649114173228397"/>
+          <c:w val="0.45224299065420598"/>
+          <c:h val="5.36224946313529E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3699,7 +3725,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3729,7 +3755,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3741,9 +3767,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3784,8 +3810,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.348250442643481"/>
-          <c:y val="0.0278770249260244"/>
+          <c:x val="0.34825044264348098"/>
+          <c:y val="2.78770249260244E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3813,7 +3839,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3826,8 +3852,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.105080683470325"/>
           <c:y val="0.12565749235474"/>
-          <c:w val="0.85864874980207"/>
-          <c:h val="0.706955301994436"/>
+          <c:w val="0.85864874980206995"/>
+          <c:h val="0.70695530199443601"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3886,7 +3912,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.131590781499662"/>
-                  <c:y val="-0.595944881889764"/>
+                  <c:y val="-0.59594488188976402"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3914,7 +3940,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3926,25 +3952,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3956,30 +3982,35 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.938</c:v>
+                  <c:v>7.9379999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.616</c:v>
+                  <c:v>7.6159999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.428</c:v>
+                  <c:v>7.4279999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.924</c:v>
+                  <c:v>6.9240000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6.532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.478</c:v>
+                  <c:v>6.4779999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.334</c:v>
+                  <c:v>6.3339999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8D75-7E4C-B780-013989DBE889}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4048,8 +4079,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.443103110740042"/>
-              <c:y val="0.889080510646228"/>
+              <c:x val="0.44310311074004199"/>
+              <c:y val="0.88908051064622795"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4077,10 +4108,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4114,7 +4146,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222471680"/>
@@ -4125,7 +4157,7 @@
         <c:axId val="-1222471680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6.0"/>
+          <c:min val="6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4178,8 +4210,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0164533820840951"/>
-              <c:y val="0.319635676274411"/>
+              <c:x val="1.6453382084095101E-2"/>
+              <c:y val="0.31963567627441097"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4207,7 +4239,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4245,7 +4277,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-1222467152"/>
@@ -4266,10 +4298,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.291636125466035"/>
-          <c:y val="0.932322135768532"/>
-          <c:w val="0.442321755027422"/>
-          <c:h val="0.0558435447048409"/>
+          <c:x val="0.29163612546603501"/>
+          <c:y val="0.93232213576853196"/>
+          <c:w val="0.44232175502742199"/>
+          <c:h val="5.5843544704840903E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4297,7 +4329,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4327,7 +4359,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4339,9 +4371,9 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4390,8 +4422,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4419,7 +4451,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4430,10 +4462,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.138501216618556"/>
+          <c:x val="0.13850121661855599"/>
           <c:y val="0.12840625"/>
-          <c:w val="0.823418169177989"/>
-          <c:h val="0.641036171259842"/>
+          <c:w val="0.82341816917798905"/>
+          <c:h val="0.64103617125984202"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4491,8 +4523,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.034970906947572"/>
-                  <c:y val="-0.0272659940944882"/>
+                  <c:x val="-3.4970906947572003E-2"/>
+                  <c:y val="-2.72659940944882E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4520,7 +4552,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4532,25 +4564,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4565,27 +4597,32 @@
                   <c:v>142.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>315.696</c:v>
+                  <c:v>315.69600000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>668.373</c:v>
+                  <c:v>668.37300000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1225.67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2110.207</c:v>
+                  <c:v>2110.2069999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3655.033</c:v>
+                  <c:v>3655.0329999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4841.168</c:v>
+                  <c:v>4841.1679999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B7F2-5848-9AB2-4CFE0FE6FA45}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4654,8 +4691,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.431803990520602"/>
-              <c:y val="0.838081938976378"/>
+              <c:x val="0.43180399052060198"/>
+              <c:y val="0.83808193897637795"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4683,7 +4720,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4721,7 +4758,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-878423312"/>
@@ -4784,8 +4821,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0153550863723608"/>
-              <c:y val="0.279010334645669"/>
+              <c:x val="1.5355086372360801E-2"/>
+              <c:y val="0.27901033464566899"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4813,11 +4850,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4851,7 +4888,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-878289072"/>
@@ -4872,10 +4909,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.274009853854641"/>
+          <c:x val="0.27400985385464099"/>
           <c:y val="0.906640255905512"/>
-          <c:w val="0.464395393474088"/>
-          <c:h val="0.0589847440944882"/>
+          <c:w val="0.46439539347408798"/>
+          <c:h val="5.8984744094488201E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4903,7 +4940,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4933,7 +4970,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4945,9 +4982,9 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4988,8 +5025,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.326312593278781"/>
-          <c:y val="0.0342465753424657"/>
+          <c:x val="0.32631259327878098"/>
+          <c:y val="3.4246575342465703E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5017,7 +5054,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5028,10 +5065,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118685586598972"/>
+          <c:x val="0.11868558659897201"/>
           <c:y val="0.12840625"/>
-          <c:w val="0.843013255099869"/>
-          <c:h val="0.641036171259842"/>
+          <c:w val="0.84301325509986902"/>
+          <c:h val="0.64103617125984202"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5089,8 +5126,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.121055543732709"/>
-                  <c:y val="-0.419776820866142"/>
+                  <c:x val="0.12105554373270901"/>
+                  <c:y val="-0.41977682086614199"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5118,7 +5155,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5130,25 +5167,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5160,13 +5197,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.809</c:v>
+                  <c:v>5.8090000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.796</c:v>
+                  <c:v>5.7960000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.791</c:v>
+                  <c:v>5.7910000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.23</c:v>
@@ -5178,12 +5215,17 @@
                   <c:v>4.72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.69</c:v>
+                  <c:v>4.6900000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5470-694D-83B7-3746BAEA7440}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5252,8 +5294,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.426226248745934"/>
-              <c:y val="0.841206938976378"/>
+              <c:x val="0.42622624874593401"/>
+              <c:y val="0.84120693897637799"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5281,10 +5323,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5318,7 +5361,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-877999840"/>
@@ -5329,7 +5372,7 @@
         <c:axId val="-877999840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="4.0"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5382,8 +5425,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0231660231660232"/>
-              <c:y val="0.276822834645669"/>
+              <c:x val="2.31660231660232E-2"/>
+              <c:y val="0.27682283464566898"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5411,7 +5454,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5449,7 +5492,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-878003232"/>
@@ -5470,10 +5513,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.299592618490256"/>
-          <c:y val="0.897265255905512"/>
+          <c:x val="0.29959261849025598"/>
+          <c:y val="0.89726525590551198"/>
           <c:w val="0.467084942084942"/>
-          <c:h val="0.0589847440944882"/>
+          <c:h val="5.8984744094488201E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5501,7 +5544,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5531,7 +5574,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5543,9 +5586,9 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5594,8 +5637,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.352908359859273"/>
-          <c:y val="0.0369131758530184"/>
+          <c:x val="0.35290835985927299"/>
+          <c:y val="3.6913175853018398E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5623,7 +5666,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5636,8 +5679,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.121629669961468"/>
           <c:y val="0.109573333333333"/>
-          <c:w val="0.843193025073993"/>
-          <c:h val="0.693684199475066"/>
+          <c:w val="0.84319302507399296"/>
+          <c:h val="0.69368419947506599"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5693,7 +5736,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5719,7 +5761,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES_tradnl"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -5731,25 +5773,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5761,10 +5803,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>39.169</c:v>
+                  <c:v>39.168999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.127</c:v>
+                  <c:v>66.126999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>120.419</c:v>
@@ -5776,15 +5818,20 @@
                   <c:v>351.548</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>629.475</c:v>
+                  <c:v>629.47500000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>778.706</c:v>
+                  <c:v>778.70600000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4E44-C64F-8075-7C302405DB36}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5853,8 +5900,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.420824956720835"/>
-              <c:y val="0.858832125984252"/>
+              <c:x val="0.42082495672083498"/>
+              <c:y val="0.85883212598425196"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5882,10 +5929,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5919,7 +5967,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-936523936"/>
@@ -5982,8 +6030,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0195035460992908"/>
-              <c:y val="0.308755485564304"/>
+              <c:x val="1.9503546099290801E-2"/>
+              <c:y val="0.30875548556430399"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6011,7 +6059,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES_tradnl"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6049,7 +6097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES_tradnl"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="-936527056"/>
@@ -6066,7 +6114,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6092,7 +6139,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES_tradnl"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6122,7 +6169,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES_tradnl"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11710,7 +11757,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11742,7 +11795,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11779,7 +11838,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11811,7 +11876,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11848,7 +11919,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11880,7 +11957,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11917,7 +12000,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11949,7 +12038,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11986,7 +12081,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -12018,7 +12119,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -12334,11 +12441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12898,11 +13005,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12913,10 +13020,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
@@ -12945,10 +13052,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
@@ -12960,10 +13067,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -13326,10 +13433,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A4:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>

</xml_diff>